<commit_message>
added total cruise otoliths and prop. of hauls > 30 otoliths plots
</commit_message>
<xml_diff>
--- a/data/AI_core_collections.xlsx
+++ b/data/AI_core_collections.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="68">
   <si>
     <t>SBS</t>
   </si>
@@ -227,6 +227,9 @@
   </si>
   <si>
     <t>pollock collection</t>
+  </si>
+  <si>
+    <t>no_vessels</t>
   </si>
 </sst>
 </file>
@@ -553,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="149" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -565,16 +568,17 @@
     <col min="2" max="2" width="32.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.54296875" customWidth="1"/>
-    <col min="11" max="11" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.26953125" customWidth="1"/>
+    <col min="6" max="6" width="3.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.54296875" customWidth="1"/>
+    <col min="12" max="12" width="14.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -588,28 +592,31 @@
         <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
       <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
         <v>58</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>59</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>10110</v>
       </c>
@@ -622,7 +629,7 @@
       <c r="D2">
         <v>500</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2">
         <v>3</v>
       </c>
       <c r="F2" s="1">
@@ -634,17 +641,20 @@
       <c r="H2" s="1">
         <v>3</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1">
+        <v>3</v>
+      </c>
+      <c r="J2" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="1">
-        <v>10</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="K2" s="1">
+        <v>10</v>
+      </c>
+      <c r="L2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>21921</v>
       </c>
@@ -658,7 +668,7 @@
         <v>1000</v>
       </c>
       <c r="E3">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F3">
         <v>10</v>
@@ -669,17 +679,20 @@
       <c r="H3">
         <v>10</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3" t="s">
         <v>60</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>30052</v>
       </c>
@@ -693,7 +706,7 @@
         <v>400</v>
       </c>
       <c r="E4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F4">
         <v>8</v>
@@ -704,17 +717,20 @@
       <c r="H4">
         <v>8</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4">
+        <v>8</v>
+      </c>
+      <c r="J4" t="s">
         <v>60</v>
       </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>30152</v>
       </c>
@@ -724,29 +740,35 @@
       <c r="C5" t="s">
         <v>24</v>
       </c>
+      <c r="D5">
+        <v>100</v>
+      </c>
       <c r="E5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H5">
-        <v>5</v>
-      </c>
-      <c r="I5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5">
+        <v>8</v>
+      </c>
+      <c r="J5" t="s">
         <v>60</v>
       </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>10115</v>
       </c>
@@ -760,7 +782,7 @@
         <v>200</v>
       </c>
       <c r="E6">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="F6">
         <v>15</v>
@@ -771,17 +793,20 @@
       <c r="H6">
         <v>15</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6">
+        <v>15</v>
+      </c>
+      <c r="J6" t="s">
         <v>60</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>30535</v>
       </c>
@@ -791,6 +816,9 @@
       <c r="C7" t="s">
         <v>29</v>
       </c>
+      <c r="D7">
+        <v>50</v>
+      </c>
       <c r="E7">
         <v>3</v>
       </c>
@@ -803,17 +831,20 @@
       <c r="H7">
         <v>3</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7" t="s">
         <v>60</v>
       </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>10112</v>
       </c>
@@ -838,17 +869,20 @@
       <c r="H8">
         <v>3</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8">
+        <v>3</v>
+      </c>
+      <c r="J8" t="s">
         <v>60</v>
       </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>30420</v>
       </c>
@@ -862,7 +896,7 @@
         <v>700</v>
       </c>
       <c r="E9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F9">
         <v>5</v>
@@ -873,17 +907,20 @@
       <c r="H9">
         <v>5</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9">
+        <v>5</v>
+      </c>
+      <c r="J9" t="s">
         <v>57</v>
       </c>
-      <c r="J9">
-        <v>5</v>
-      </c>
-      <c r="K9" t="s">
+      <c r="K9">
+        <v>5</v>
+      </c>
+      <c r="L9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>10261</v>
       </c>
@@ -894,10 +931,10 @@
         <v>46</v>
       </c>
       <c r="D10">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="E10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F10">
         <v>2</v>
@@ -908,17 +945,20 @@
       <c r="H10">
         <v>2</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10" t="s">
         <v>57</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>2</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>21720</v>
       </c>
@@ -943,17 +983,20 @@
       <c r="H11">
         <v>3</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="J11" t="s">
         <v>60</v>
       </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>30060</v>
       </c>
@@ -967,7 +1010,7 @@
         <v>1200</v>
       </c>
       <c r="E12">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F12">
         <v>5</v>
@@ -978,17 +1021,20 @@
       <c r="H12">
         <v>5</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12">
+        <v>5</v>
+      </c>
+      <c r="J12" t="s">
         <v>57</v>
       </c>
-      <c r="J12">
-        <v>5</v>
-      </c>
-      <c r="K12" t="s">
+      <c r="K12">
+        <v>5</v>
+      </c>
+      <c r="L12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>30051</v>
       </c>
@@ -1002,7 +1048,7 @@
         <v>100</v>
       </c>
       <c r="E13">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F13">
         <v>10</v>
@@ -1013,17 +1059,20 @@
       <c r="H13">
         <v>10</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13">
+        <v>10</v>
+      </c>
+      <c r="J13" t="s">
         <v>60</v>
       </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13" t="s">
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>30576</v>
       </c>
@@ -1037,28 +1086,31 @@
         <v>350</v>
       </c>
       <c r="E14">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F14">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G14">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="H14">
-        <v>8</v>
-      </c>
-      <c r="I14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14">
+        <v>12</v>
+      </c>
+      <c r="J14" t="s">
         <v>60</v>
       </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14" t="s">
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>30020</v>
       </c>
@@ -1068,29 +1120,35 @@
       <c r="C15" t="s">
         <v>40</v>
       </c>
+      <c r="D15">
+        <v>400</v>
+      </c>
       <c r="E15">
         <v>3</v>
       </c>
       <c r="F15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H15">
-        <v>3</v>
-      </c>
-      <c r="I15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15">
+        <v>4</v>
+      </c>
+      <c r="J15" t="s">
         <v>60</v>
       </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15" t="s">
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>10262</v>
       </c>
@@ -1104,28 +1162,31 @@
         <v>300</v>
       </c>
       <c r="E16">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F16">
         <v>10</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
         <v>60</v>
       </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16" t="s">
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>21740</v>
       </c>
@@ -1138,7 +1199,10 @@
       <c r="D17">
         <v>700</v>
       </c>
-      <c r="K17" t="s">
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="L17" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1355,8 +1419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L19" sqref="A19:L19"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1483,7 +1547,7 @@
         <v>60</v>
       </c>
       <c r="K3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L3" t="s">
         <v>51</v>
@@ -1553,7 +1617,7 @@
         <v>60</v>
       </c>
       <c r="K5">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="L5" t="s">
         <v>53</v>
@@ -1915,7 +1979,7 @@
         <v>60</v>
       </c>
       <c r="K15">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L15" t="s">
         <v>53</v>
@@ -2017,7 +2081,7 @@
         <v>60</v>
       </c>
       <c r="K18">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L18" t="s">
         <v>55</v>

</xml_diff>